<commit_message>
add unit-tests in xls(have errors), add unit-tests(8/25)
</commit_message>
<xml_diff>
--- a/Aspekty.xlsx
+++ b/Aspekty.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\programming labs\11_Tarapatina_E_S\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA3DD63-CA5D-4EBA-9DFB-64FA6F0F0FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Аспекты тестирования" sheetId="2" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>Аспекты тестирования функции</t>
   </si>
@@ -128,14 +122,13 @@
     </r>
   </si>
   <si>
-    <t>void count();
+    <t>void count()
+{
+int a = 0;
+}
 int main()
 {
 count();
-}
-void count()
-{
-  int a = 0;
 }</t>
   </si>
   <si>
@@ -146,6 +139,9 @@
   </si>
   <si>
     <t>Наименование</t>
+  </si>
+  <si>
+    <t>Имя функции функции</t>
   </si>
   <si>
     <t xml:space="preserve"> Количество строк в исходном коде</t>
@@ -181,29 +177,56 @@
     <t>Типовой тест с неверным вызовом функции</t>
   </si>
   <si>
+    <t>void count()                                                                            {                                                                                                  int a = 0;                                                                                    }                                                                                                 int main()
+{
+int a = 0;
+a = count();                                                                               return 0;
+}</t>
+  </si>
+  <si>
     <t>Типовой тест без вызова функции</t>
+  </si>
+  <si>
+    <t>void count()                                                                            {                                                                                                  int a = 0;                                                                                    }                                                                                                 int main()
+{
+int a = 0;
+return 0;
+}</t>
   </si>
   <si>
     <t>Функция возвращает значение</t>
   </si>
   <si>
-    <t>Неверный вызов функции, которая возвращает значение</t>
+    <t>int count()
+{                                                                                                  int a = 0;
+return a;                                                                                    }                                                                                                 int main()
+{
+int a = 0;
+a = count();
+return 0;
+}</t>
   </si>
   <si>
-    <t xml:space="preserve">int main()
+    <t>Вызов функции, которая возвращает значение, но оно не используется</t>
+  </si>
+  <si>
+    <t>int count()
+{                                                                                                  int a = 0;
+return a;                                                                                    }                                                                                                 int main()
 {
-cout();
-}
-</t>
+int a = 0;
+count();
+return 0;
+}</t>
   </si>
   <si>
     <t>Функция имеет аргументы</t>
   </si>
   <si>
-    <t>int main()
+    <t>void count(int b)                                                                            {                                                                                                  int a = 0;                                                                                    }                                                                                                 int main()
 {
-int a = 0;
-count(a);
+count();
+return 0;
 }</t>
   </si>
   <si>
@@ -213,83 +236,11 @@
     <t>функция вызывается внутри if()</t>
   </si>
   <si>
-    <t>Функция вызывается внутри for()</t>
-  </si>
-  <si>
-    <t>int main()
-{
- int i = 0;
-for(i; i &lt; 23; i++)
-{
-    count(i);
-}
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Функция вызывется внутри while() </t>
-  </si>
-  <si>
-    <t>int main()
-{ 
-int a = 0;
-while(a &lt; 10)
-{
-    count(i);
-}
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Функция вызывется внутри do{}while(); </t>
-  </si>
-  <si>
-    <t>int main()
-{ 
-int a = 0;
-do
-{
-    count(i);
-}while(a &lt; 10);
-}</t>
-  </si>
-  <si>
-    <t>функция вызывается внутри if(){}else{}</t>
-  </si>
-  <si>
-    <t>int main()
+    <t xml:space="preserve"> void count()
 {
 int a = 0;
-if(a == 0)
-{
-   a = 1;
-}
-else
-{
-  count();
-}
-}</t>
-  </si>
-  <si>
-    <t>Имя функции функции</t>
-  </si>
-  <si>
-    <t>void count();                                                                       int main()
-{
-int a = 0;
-a = count();                                                                               
-return 0;                                                                                  }</t>
-  </si>
-  <si>
-    <t>void count();                                                                       int main()
-{
-int a = 0;                                                                         return 0;
-}</t>
-  </si>
-  <si>
-    <t>void count();                                                                       int main()                                                                                 {                                                                                                       int a = 0;
-a = count();                                                                         return 0;                                                                                  }</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> void count(){}                                                                      int main()
+}  
+int main()
 {
 int a = 0;
 if(a == 0)
@@ -299,24 +250,172 @@
 }</t>
   </si>
   <si>
-    <t>void count()                                                                            {                                                                                                  int a = 0;                                                                                    }                                                                                              int main()
+    <t>Функция вызывается внутри for()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
 {
-count();
+int a = 0;
+}  
+int main()
+{
+ int i = 0;
+for(i; i &lt; 23; i++)
+{
+    count(-2);
+}
 }</t>
   </si>
   <si>
-    <t>void count()                                                                            {                                                                                                  int a = 0;                                                                                    }                                                                                                 int main()
+    <t xml:space="preserve">Функция вызывется внутри while() </t>
+  </si>
+  <si>
+    <t>void count(int a)                                                                            {                                                                                                   a = 0;                                                                                   
+}
+int main()
+{ 
+int a = 0;
+while(a &lt; 10)
+{
+    count(a);
+}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Функция вызывется внутри do{}while(); </t>
+  </si>
+  <si>
+    <t>void count()                                                                            {                                                                                                  int a = 0;                                                                                    }
+int main()
+{ 
+int a = 0;
+do
+{
+    count();
+}while(a &lt; 10);
+}</t>
+  </si>
+  <si>
+    <t>функция вызывается внутри if(){}else{}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
 {
 int a = 0;
-a = count();                                                                               return 0;
+}  
+int main()
+{
+int a = 0;
+if(a == 0)
+{
+   a = 1;
+}
+else
+{
+  count(5);
+}
+}</t>
+  </si>
+  <si>
+    <t>Объявлена не только исходная пользовательская фукнция</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> count</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
+{
+int a = 0;
+}
+void minus()
+{
+int b = 0;  
+}
+int main()
+{
+int i = 0;
+count(1);
+}</t>
+  </si>
+  <si>
+    <t>Объявлена и используется не только исходная пользовательская фукнция</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
+{
+int a = 0;
+}
+void minus()
+{
+int b = 0;  
+}
+int main()
+{
+int i = 0;
+minus();
+count(34);
+}</t>
+  </si>
+  <si>
+    <t>Объявлена и используется не только исходная пользовательская фукнция(исходная функция не используется)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
+{
+int a = 0;
+}
+void minus()
+{
+int b = 0;  
+}
+int main()
+{
+int i = 0;
+minus();
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Исходная функция используется более одного раза</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
+{
+int a = 0;
+}
+int main()
+{
+int i = 0;
+count();
+count(40);
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Исходная функция неверно используется более одного раза</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> void count()
+{
+int a = 0;
+}
+int main()
+{
+int i = 0;
+count(10);
+count(40);
 }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="45">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -385,6 +484,12 @@
     <font>
       <b/>
       <sz val="18"/>
+      <name val="Consolas"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <name val="Arial"/>
       <charset val="204"/>
     </font>
@@ -403,6 +508,12 @@
     </font>
     <font>
       <sz val="18"/>
+      <color indexed="16"/>
+      <name val="Consolas"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="204"/>
@@ -410,7 +521,6 @@
     </font>
     <font>
       <sz val="18"/>
-      <color indexed="16"/>
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -452,42 +562,358 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color indexed="16"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -510,120 +936,399 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="41"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="20% — Акцент3" xfId="1" builtinId="38"/>
+    <cellStyle name="Денежный [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% — Акцент5" xfId="3" builtinId="47"/>
+    <cellStyle name="Хороший" xfId="4" builtinId="26"/>
+    <cellStyle name="Запятая [0]" xfId="5" builtinId="6"/>
+    <cellStyle name="Денежный" xfId="6" builtinId="4"/>
+    <cellStyle name="Запятая" xfId="7" builtinId="3"/>
+    <cellStyle name="40% — Акцент6" xfId="8" builtinId="51"/>
+    <cellStyle name="Процент" xfId="9" builtinId="5"/>
+    <cellStyle name="20% — Акцент2" xfId="10" builtinId="34"/>
+    <cellStyle name="Итого" xfId="11" builtinId="25"/>
+    <cellStyle name="Вывод" xfId="12" builtinId="21"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8"/>
+    <cellStyle name="Примечание" xfId="14" builtinId="10"/>
+    <cellStyle name="40% — Акцент4" xfId="15" builtinId="43"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9"/>
+    <cellStyle name="Предупреждающий текст" xfId="17" builtinId="11"/>
+    <cellStyle name="Заголовок" xfId="18" builtinId="15"/>
+    <cellStyle name="Пояснительный текст" xfId="19" builtinId="53"/>
+    <cellStyle name="Заголовок 1" xfId="20" builtinId="16"/>
+    <cellStyle name="Заголовок 2" xfId="21" builtinId="17"/>
+    <cellStyle name="Заголовок 3" xfId="22" builtinId="18"/>
+    <cellStyle name="Заголовок 4" xfId="23" builtinId="19"/>
+    <cellStyle name="Ввод" xfId="24" builtinId="20"/>
+    <cellStyle name="Проверить ячейку" xfId="25" builtinId="23"/>
+    <cellStyle name="Вычисление" xfId="26" builtinId="22"/>
+    <cellStyle name="Связанная ячейка" xfId="27" builtinId="24"/>
+    <cellStyle name="Плохой" xfId="28" builtinId="27"/>
+    <cellStyle name="Акцент5" xfId="29" builtinId="45"/>
+    <cellStyle name="Нейтральный" xfId="30" builtinId="28"/>
+    <cellStyle name="Акцент1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% — Акцент1" xfId="32" builtinId="30"/>
+    <cellStyle name="40% — Акцент1" xfId="33" builtinId="31"/>
+    <cellStyle name="20% — Акцент5" xfId="34" builtinId="46"/>
+    <cellStyle name="60% — Акцент1" xfId="35" builtinId="32"/>
+    <cellStyle name="Акцент2" xfId="36" builtinId="33"/>
+    <cellStyle name="40% — Акцент2" xfId="37" builtinId="35"/>
+    <cellStyle name="20% — Акцент6" xfId="38" builtinId="50"/>
+    <cellStyle name="60% — Акцент2" xfId="39" builtinId="36"/>
+    <cellStyle name="Акцент3" xfId="40" builtinId="37"/>
+    <cellStyle name="Обычный 2" xfId="41"/>
+    <cellStyle name="40% — Акцент3" xfId="42" builtinId="39"/>
+    <cellStyle name="60% — Акцент3" xfId="43" builtinId="40"/>
+    <cellStyle name="Акцент4" xfId="44" builtinId="41"/>
+    <cellStyle name="20% — Акцент4" xfId="45" builtinId="42"/>
+    <cellStyle name="60% — Акцент4" xfId="46" builtinId="44"/>
+    <cellStyle name="60% — Акцент5" xfId="47" builtinId="48"/>
+    <cellStyle name="Акцент6" xfId="48" builtinId="49"/>
+    <cellStyle name="60% — Акцент6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -908,25 +1613,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:IV21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="74.6640625" customWidth="1"/>
-    <col min="2" max="2" width="72.83203125" customWidth="1"/>
+    <col min="1" max="1" width="74.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="72.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" ht="23.25" spans="1:256">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,41 +1873,41 @@
       <c r="IC1" s="10"/>
       <c r="ID1" s="10"/>
       <c r="IE1" s="10"/>
-      <c r="IF1" s="24"/>
-      <c r="IG1" s="24"/>
-      <c r="IH1" s="24"/>
-      <c r="II1" s="24"/>
-      <c r="IJ1" s="24"/>
-      <c r="IK1" s="24"/>
-      <c r="IL1" s="24"/>
-      <c r="IM1" s="24"/>
-      <c r="IN1" s="24"/>
-      <c r="IO1" s="24"/>
-      <c r="IP1" s="24"/>
-      <c r="IQ1" s="24"/>
-      <c r="IR1" s="24"/>
-      <c r="IS1" s="24"/>
+      <c r="IF1" s="25"/>
+      <c r="IG1" s="25"/>
+      <c r="IH1" s="25"/>
+      <c r="II1" s="25"/>
+      <c r="IJ1" s="25"/>
+      <c r="IK1" s="25"/>
+      <c r="IL1" s="25"/>
+      <c r="IM1" s="25"/>
+      <c r="IN1" s="25"/>
+      <c r="IO1" s="25"/>
+      <c r="IP1" s="25"/>
+      <c r="IQ1" s="25"/>
+      <c r="IR1" s="25"/>
+      <c r="IS1" s="25"/>
       <c r="IT1" s="10"/>
       <c r="IU1" s="10"/>
       <c r="IV1" s="10"/>
     </row>
-    <row r="2" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" ht="23.25" spans="1:256">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
@@ -1446,23 +2151,23 @@
       <c r="IU2" s="10"/>
       <c r="IV2" s="10"/>
     </row>
-    <row r="3" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" ht="23.25" spans="1:256">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
@@ -1706,7 +2411,7 @@
       <c r="IU3" s="10"/>
       <c r="IV3" s="10"/>
     </row>
-    <row r="4" spans="1:256" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1964,11 +2669,11 @@
       <c r="IU4" s="10"/>
       <c r="IV4" s="10"/>
     </row>
-    <row r="5" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+    <row r="5" ht="23.25" spans="1:256">
+      <c r="A5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="10"/>
@@ -2226,11 +2931,11 @@
       <c r="IU5" s="10"/>
       <c r="IV5" s="10"/>
     </row>
-    <row r="6" spans="1:256" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+    <row r="6" ht="23.25" spans="1:256">
+      <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="10"/>
@@ -2488,11 +3193,11 @@
       <c r="IU6" s="10"/>
       <c r="IV6" s="10"/>
     </row>
-    <row r="7" spans="1:256" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+    <row r="7" ht="23.1" customHeight="1" spans="1:256">
+      <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10"/>
@@ -2750,11 +3455,11 @@
       <c r="IU7" s="10"/>
       <c r="IV7" s="10"/>
     </row>
-    <row r="8" spans="1:256" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+    <row r="8" ht="23.25" spans="1:256">
+      <c r="A8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="10"/>
@@ -3012,11 +3717,11 @@
       <c r="IU8" s="10"/>
       <c r="IV8" s="10"/>
     </row>
-    <row r="9" spans="1:256" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+    <row r="9" ht="23.25" spans="1:256">
+      <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="10"/>
@@ -3274,11 +3979,11 @@
       <c r="IU9" s="10"/>
       <c r="IV9" s="10"/>
     </row>
-    <row r="10" spans="1:256" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+    <row r="10" ht="46.5" spans="1:256">
+      <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="10"/>
@@ -3536,11 +4241,11 @@
       <c r="IU10" s="10"/>
       <c r="IV10" s="10"/>
     </row>
-    <row r="11" spans="1:256" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+    <row r="11" ht="23.25" spans="1:256">
+      <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="10"/>
@@ -3798,11 +4503,11 @@
       <c r="IU11" s="10"/>
       <c r="IV11" s="10"/>
     </row>
-    <row r="12" spans="1:256" ht="46.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+    <row r="12" ht="46.5" spans="1:256">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="10"/>
@@ -4060,92 +4765,94 @@
       <c r="IU12" s="10"/>
       <c r="IV12" s="10"/>
     </row>
-    <row r="13" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
+    <row r="13" ht="23.25" spans="1:2">
+      <c r="A13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="32" t="s">
+    <row r="14" ht="23.25" spans="1:2">
+      <c r="A14" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:256" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+    <row r="15" ht="46.5" spans="1:2">
+      <c r="A15" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" ht="23.25" spans="1:2">
       <c r="A16" s="3"/>
-      <c r="B16" s="34"/>
+      <c r="B16" s="36"/>
     </row>
-    <row r="17" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="23"/>
+    <row r="17" ht="23.25" spans="1:2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
+    <row r="18" ht="23.25" spans="1:2">
+      <c r="A18" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="19" ht="23.25" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" ht="23.25" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="209.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+    <row r="21" ht="186" spans="1:2">
+      <c r="A21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:IV51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="84.83203125" customWidth="1"/>
-    <col min="2" max="2" width="108.83203125" customWidth="1"/>
-    <col min="3" max="3" width="73.33203125" customWidth="1"/>
-    <col min="4" max="4" width="84.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col min="1" max="1" width="84.8333333333333" customWidth="1"/>
+    <col min="2" max="2" width="108.833333333333" customWidth="1"/>
+    <col min="3" max="3" width="73.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="84.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="37.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" ht="23.25" spans="1:256">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -4387,25 +5094,25 @@
       <c r="IC1" s="3"/>
       <c r="ID1" s="3"/>
       <c r="IE1" s="3"/>
-      <c r="IF1" s="24"/>
-      <c r="IG1" s="24"/>
-      <c r="IH1" s="24"/>
-      <c r="II1" s="24"/>
-      <c r="IJ1" s="24"/>
-      <c r="IK1" s="24"/>
-      <c r="IL1" s="24"/>
-      <c r="IM1" s="24"/>
-      <c r="IN1" s="24"/>
-      <c r="IO1" s="24"/>
-      <c r="IP1" s="24"/>
-      <c r="IQ1" s="24"/>
-      <c r="IR1" s="24"/>
-      <c r="IS1" s="24"/>
+      <c r="IF1" s="25"/>
+      <c r="IG1" s="25"/>
+      <c r="IH1" s="25"/>
+      <c r="II1" s="25"/>
+      <c r="IJ1" s="25"/>
+      <c r="IK1" s="25"/>
+      <c r="IL1" s="25"/>
+      <c r="IM1" s="25"/>
+      <c r="IN1" s="25"/>
+      <c r="IO1" s="25"/>
+      <c r="IP1" s="25"/>
+      <c r="IQ1" s="25"/>
+      <c r="IR1" s="25"/>
+      <c r="IS1" s="25"/>
       <c r="IT1" s="10"/>
       <c r="IU1" s="10"/>
       <c r="IV1" s="10"/>
     </row>
-    <row r="2" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" ht="23.25" spans="1:256">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4665,7 +5372,7 @@
       <c r="IU2" s="10"/>
       <c r="IV2" s="10"/>
     </row>
-    <row r="3" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" ht="23.25" spans="1:256">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -4925,7 +5632,7 @@
       <c r="IU3" s="10"/>
       <c r="IV3" s="10"/>
     </row>
-    <row r="4" spans="1:256" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -5183,21 +5890,21 @@
       <c r="IU4" s="10"/>
       <c r="IV4" s="10"/>
     </row>
-    <row r="5" spans="1:256" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" ht="23.25" spans="1:256">
       <c r="A5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>35</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -5451,21 +6158,21 @@
       <c r="IU5" s="10"/>
       <c r="IV5" s="10"/>
     </row>
-    <row r="6" spans="1:256" ht="162.75" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="39" t="s">
+    <row r="6" ht="186" spans="1:256">
+      <c r="A6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="14">
-        <v>6</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="14">
-        <v>-2</v>
+      <c r="C6" s="15">
+        <v>8</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15">
+        <v>-1</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -5719,20 +6426,20 @@
       <c r="IU6" s="10"/>
       <c r="IV6" s="10"/>
     </row>
-    <row r="7" spans="1:256" ht="232.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="39" t="s">
+    <row r="7" ht="232.5" spans="1:256">
+      <c r="A7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17">
-        <v>2</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="14">
+      <c r="C7" s="19">
+        <v>10</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="15">
         <v>2</v>
       </c>
       <c r="F7" s="10"/>
@@ -5987,21 +6694,21 @@
       <c r="IU7" s="10"/>
       <c r="IV7" s="10"/>
     </row>
-    <row r="8" spans="1:256" ht="139.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="39" t="s">
+    <row r="8" ht="209.25" spans="1:256">
+      <c r="A8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="14">
-        <v>1</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="14">
-        <v>-1</v>
+      <c r="C8" s="15">
+        <v>9</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="15">
+        <v>-2</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -6255,21 +6962,21 @@
       <c r="IU8" s="10"/>
       <c r="IV8" s="10"/>
     </row>
-    <row r="9" spans="1:256" ht="162.75" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="39" t="s">
+    <row r="9" ht="255.75" spans="1:256">
+      <c r="A9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="14">
-        <v>2</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="14">
-        <v>-2</v>
+      <c r="C9" s="15">
+        <v>11</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="15">
+        <v>-1</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -6523,21 +7230,21 @@
       <c r="IU9" s="10"/>
       <c r="IV9" s="10"/>
     </row>
-    <row r="10" spans="1:256" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="39" t="s">
+    <row r="10" ht="255.75" spans="1:256">
+      <c r="A10" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
+      <c r="C10" s="15">
+        <v>11</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="15">
+        <v>-1</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -6791,21 +7498,21 @@
       <c r="IU10" s="10"/>
       <c r="IV10" s="10"/>
     </row>
-    <row r="11" spans="1:256" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="39" t="s">
+    <row r="11" ht="209.25" spans="1:256">
+      <c r="A11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="21">
         <v>2</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="19">
-        <v>-2</v>
+        <v>47</v>
+      </c>
+      <c r="E11" s="21">
+        <v>-1</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -7059,21 +7766,21 @@
       <c r="IU11" s="3"/>
       <c r="IV11" s="3"/>
     </row>
-    <row r="12" spans="1:256" ht="186" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="39" t="s">
+    <row r="12" ht="209.25" spans="1:256">
+      <c r="A12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="19">
-        <v>1</v>
+      <c r="C12" s="21">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="21">
+        <v>7</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -7327,21 +8034,21 @@
       <c r="IU12" s="3"/>
       <c r="IV12" s="3"/>
     </row>
-    <row r="13" spans="1:256" ht="209.25" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="39" t="s">
+    <row r="13" ht="279" spans="1:256">
+      <c r="A13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="14">
-        <v>5</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="19">
-        <v>-2</v>
+      <c r="C13" s="15">
+        <v>12</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="21">
+        <v>-1</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -7595,21 +8302,21 @@
       <c r="IU13" s="3"/>
       <c r="IV13" s="3"/>
     </row>
-    <row r="14" spans="1:256" ht="186" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="39" t="s">
+    <row r="14" ht="279" spans="1:256">
+      <c r="A14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="19">
-        <v>5</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="19">
-        <v>4</v>
+      <c r="C14" s="21">
+        <v>12</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="21">
+        <v>10</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -7863,21 +8570,21 @@
       <c r="IU14" s="3"/>
       <c r="IV14" s="3"/>
     </row>
-    <row r="15" spans="1:256" ht="186" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="39" t="s">
+    <row r="15" ht="279" spans="1:256">
+      <c r="A15" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="19">
-        <v>5</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="19">
-        <v>4</v>
+      <c r="C15" s="21">
+        <v>12</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="21">
+        <v>10</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -8131,21 +8838,21 @@
       <c r="IU15" s="3"/>
       <c r="IV15" s="3"/>
     </row>
-    <row r="16" spans="1:256" ht="186" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="39" t="s">
+    <row r="16" ht="279" spans="1:256">
+      <c r="A16" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="19">
-        <v>5</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="19">
-        <v>4</v>
+      <c r="C16" s="21">
+        <v>12</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="21">
+        <v>-1</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -8399,211 +9106,262 @@
       <c r="IU16" s="3"/>
       <c r="IV16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="279" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="39" t="s">
+    <row r="17" ht="372" spans="1:5">
+      <c r="A17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="15">
+        <v>16</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" ht="302.25" spans="1:5">
+      <c r="A18" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="19">
+        <v>13</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" ht="325.5" spans="1:5">
+      <c r="A19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="19">
+        <v>14</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" ht="302.25" spans="1:5">
+      <c r="A20" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="19">
+        <v>14</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="19">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" ht="232.5" spans="1:5">
+      <c r="A21" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="19">
+        <v>10</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="19">
         <v>9</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="19">
-        <v>-2</v>
-      </c>
     </row>
-    <row r="18" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="17"/>
+    <row r="22" ht="232.5" spans="1:5">
+      <c r="A22" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="19">
+        <v>10</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="19">
+        <v>8</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="17"/>
+    <row r="23" ht="23.25" spans="1:5">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
     </row>
-    <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="17"/>
+    <row r="24" ht="23.25" spans="1:5">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="17"/>
+    <row r="25" ht="23.25" spans="1:5">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
     </row>
-    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="17"/>
+    <row r="26" ht="23.25" spans="1:5">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
     </row>
-    <row r="23" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="17"/>
+    <row r="27" ht="23.25" spans="1:5">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
     </row>
-    <row r="24" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="17"/>
+    <row r="28" ht="23.25" spans="1:5">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
     </row>
-    <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="17"/>
+    <row r="29" ht="23.25" spans="1:5">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="17"/>
+    <row r="30" ht="23.25" spans="1:5">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="17"/>
+    <row r="31" ht="23.25" spans="1:5">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="17"/>
+    <row r="32" ht="23.25" spans="1:5">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="17"/>
+    <row r="33" ht="23.25" spans="1:5">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
     </row>
-    <row r="30" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="17"/>
+    <row r="34" ht="23.25" spans="1:4">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="18"/>
     </row>
-    <row r="31" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="17"/>
+    <row r="35" ht="23.25" spans="1:4">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="18"/>
     </row>
-    <row r="32" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="17"/>
+    <row r="36" ht="23.25" spans="1:4">
+      <c r="A36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="18"/>
     </row>
-    <row r="33" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="17"/>
+    <row r="37" ht="23.25" spans="1:4">
+      <c r="A37" s="19"/>
+      <c r="D37" s="18"/>
     </row>
-    <row r="34" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="23"/>
+    <row r="38" ht="23.25" spans="1:4">
+      <c r="A38" s="19"/>
+      <c r="D38" s="18"/>
     </row>
-    <row r="35" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="23"/>
+    <row r="39" ht="23.25" spans="1:4">
+      <c r="A39" s="19"/>
+      <c r="D39" s="18"/>
     </row>
-    <row r="36" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="23"/>
+    <row r="40" ht="23.25" spans="1:4">
+      <c r="A40" s="19"/>
+      <c r="D40" s="18"/>
     </row>
-    <row r="37" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="D37" s="23"/>
+    <row r="41" ht="23.25" spans="1:4">
+      <c r="A41" s="19"/>
+      <c r="D41" s="18"/>
     </row>
-    <row r="38" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="D38" s="23"/>
+    <row r="42" ht="23.25" spans="1:4">
+      <c r="A42" s="19"/>
+      <c r="D42" s="18"/>
     </row>
-    <row r="39" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="D39" s="23"/>
+    <row r="43" ht="23.25" spans="1:4">
+      <c r="A43" s="19"/>
+      <c r="D43" s="18"/>
     </row>
-    <row r="40" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="D40" s="23"/>
+    <row r="44" ht="23.25" spans="1:4">
+      <c r="A44" s="19"/>
+      <c r="D44" s="18"/>
     </row>
-    <row r="41" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="D41" s="23"/>
+    <row r="45" ht="23.25" spans="1:4">
+      <c r="A45" s="19"/>
+      <c r="D45" s="18"/>
     </row>
-    <row r="42" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="D42" s="23"/>
+    <row r="46" ht="23.25" spans="1:4">
+      <c r="A46" s="19"/>
+      <c r="D46" s="18"/>
     </row>
-    <row r="43" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="D43" s="23"/>
+    <row r="47" ht="23.25" spans="1:4">
+      <c r="A47" s="19"/>
+      <c r="D47" s="18"/>
     </row>
-    <row r="44" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="D44" s="23"/>
+    <row r="48" ht="23.25" spans="1:4">
+      <c r="A48" s="19"/>
+      <c r="D48" s="18"/>
     </row>
-    <row r="45" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="D45" s="23"/>
+    <row r="49" ht="23.25" spans="1:4">
+      <c r="A49" s="19"/>
+      <c r="D49" s="18"/>
     </row>
-    <row r="46" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="D46" s="23"/>
+    <row r="50" ht="23.25" spans="1:1">
+      <c r="A50" s="19"/>
     </row>
-    <row r="47" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="D47" s="23"/>
-    </row>
-    <row r="48" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
-      <c r="D48" s="23"/>
-    </row>
-    <row r="49" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="D49" s="23"/>
-    </row>
-    <row r="50" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
+    <row r="51" ht="23.25" spans="1:1">
+      <c r="A51" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>